<commit_message>
Updated info in files
</commit_message>
<xml_diff>
--- a/PCB_files/IC905_Band_Decoder_BOM-20-Jan-2025.xlsx
+++ b/PCB_files/IC905_Band_Decoder_BOM-20-Jan-2025.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9BBDB4-9589-481D-95DE-404D20F0D826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="8_{48654F1B-A63E-4FD9-B4DB-5299DF6E0C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D691DDEA-53B8-4B1C-A413-5281C816FA8F}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="1065" windowWidth="21600" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3315" yWindow="2625" windowWidth="24420" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_905_Band_Decoder_Band_Decod" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="165">
   <si>
     <t>No.</t>
   </si>
@@ -53,9 +53,6 @@
     <t>C1,C2,C3,C4,C6,C7,C8,C10,C12,C13</t>
   </si>
   <si>
-    <t>LCSC</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>1N4007</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -80,18 +74,12 @@
     <t>4</t>
   </si>
   <si>
-    <t>1N4148</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>DC-470-2.1GP</t>
-  </si>
-  <si>
     <t>DC1,DC2</t>
   </si>
   <si>
@@ -104,42 +92,21 @@
     <t>7</t>
   </si>
   <si>
-    <t>RF2622-000</t>
-  </si>
-  <si>
     <t>F1</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>B4B-XH-AM(LF)(SN)</t>
-  </si>
-  <si>
     <t>J1,J5</t>
   </si>
   <si>
-    <t>JST</t>
-  </si>
-  <si>
-    <t>C161871</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
-    <t>RCJ-042</t>
-  </si>
-  <si>
     <t>J2</t>
   </si>
   <si>
-    <t>CUI</t>
-  </si>
-  <si>
-    <t>C22359751</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -149,51 +116,21 @@
     <t>J3</t>
   </si>
   <si>
-    <t>C157925</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
-    <t>PZ254V-11-03P</t>
-  </si>
-  <si>
     <t>J4</t>
   </si>
   <si>
-    <t>XFCN(兴飞)</t>
-  </si>
-  <si>
-    <t>C2937625</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
-    <t>PJ-324</t>
-  </si>
-  <si>
     <t>J6</t>
   </si>
   <si>
-    <t>SOFNG(硕方)</t>
-  </si>
-  <si>
-    <t>C22355738</t>
-  </si>
-  <si>
     <t>13</t>
   </si>
   <si>
-    <t>XL-302UBD</t>
-  </si>
-  <si>
-    <t>XINGLIGHT(成兴光)</t>
-  </si>
-  <si>
-    <t>C2895474</t>
-  </si>
-  <si>
     <t>14</t>
   </si>
   <si>
@@ -203,33 +140,12 @@
     <t>R1</t>
   </si>
   <si>
-    <t>CFR-25JB-52-24R</t>
-  </si>
-  <si>
-    <t>YAGEO(国巨)</t>
-  </si>
-  <si>
-    <t>C1367243</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
-    <t>0Ω</t>
-  </si>
-  <si>
     <t>R2,R3,R4</t>
   </si>
   <si>
-    <t>1206W4F0000T5E</t>
-  </si>
-  <si>
-    <t>UNI-ROYAL(厚声)</t>
-  </si>
-  <si>
-    <t>C17888</t>
-  </si>
-  <si>
     <t>16</t>
   </si>
   <si>
@@ -245,51 +161,21 @@
     <t>U1</t>
   </si>
   <si>
-    <t>HTC</t>
-  </si>
-  <si>
-    <t>C411818</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
-    <t>ESP32-S3-DevKitC-1 N8</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>ULN2803AN(XBLW)</t>
-  </si>
-  <si>
     <t>U3,U4</t>
   </si>
   <si>
-    <t>XBLW(芯伯乐)</t>
-  </si>
-  <si>
-    <t>C18723560</t>
-  </si>
-  <si>
     <t>20</t>
   </si>
   <si>
-    <t>PZ2.54-2*20</t>
-  </si>
-  <si>
     <t>U5</t>
   </si>
   <si>
-    <t>ZHOURI(洲日)</t>
-  </si>
-  <si>
-    <t>C5224014</t>
-  </si>
-  <si>
     <t>21</t>
   </si>
   <si>
@@ -299,27 +185,9 @@
     <t>VR1</t>
   </si>
   <si>
-    <t>3296W-1-103LF</t>
-  </si>
-  <si>
-    <t>BOURNS</t>
-  </si>
-  <si>
-    <t>C34846</t>
-  </si>
-  <si>
     <t>HD 15-pin D-Sub, PCB mount</t>
   </si>
   <si>
-    <t>22uF electrolytic cap</t>
-  </si>
-  <si>
-    <t>10kΩ vertical top adjustment 5 or 10 turn pot</t>
-  </si>
-  <si>
-    <t>B4B-XH-AM(LF)(SN) 4-pin vertical JST-XH connector</t>
-  </si>
-  <si>
     <t>3mm dia LED - RED</t>
   </si>
   <si>
@@ -338,27 +206,9 @@
     <t>LED10G,LED144,LED430,LED1200,LED2300,LED5600</t>
   </si>
   <si>
-    <t>3-pin header</t>
-  </si>
-  <si>
-    <t>S4B-XH-A(LF)(SN) right angle 4-pin JST-XH connector</t>
-  </si>
-  <si>
-    <t>2.1x5.5 Coaxial Power jack</t>
-  </si>
-  <si>
-    <t>RF2622-000 radial resettable fuse</t>
-  </si>
-  <si>
-    <t>Phono jack (aka RCA jack), right angle PCB mount</t>
-  </si>
-  <si>
     <t>1/8" headphone audio jack</t>
   </si>
   <si>
-    <t>0Ω resistor jumper, 1206 SMD</t>
-  </si>
-  <si>
     <t>DO NOT INSTALL - 2x20 pin header, 2.54mm pitch</t>
   </si>
   <si>
@@ -392,12 +242,6 @@
     <t>https://www.digikey.com/en/products/detail/hammond-manufacturing/1455J1202BK/2360699</t>
   </si>
   <si>
-    <t>100nF radial lead</t>
-  </si>
-  <si>
-    <t>Littelfuse</t>
-  </si>
-  <si>
     <t>4609X-101-221LF-ND</t>
   </si>
   <si>
@@ -411,13 +255,268 @@
   </si>
   <si>
     <t>Bourns Inc.</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kycon-inc/KLPX-0848A-2-B/9990118</t>
+  </si>
+  <si>
+    <t>2092-KLPX-0848A-2-B-ND</t>
+  </si>
+  <si>
+    <t>Kycon, Inc.</t>
+  </si>
+  <si>
+    <t>KLPX-0848A-2-B</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/S4B-XH-A/1651041</t>
+  </si>
+  <si>
+    <t>455-2243-ND</t>
+  </si>
+  <si>
+    <t>JST Sales America Inc.</t>
+  </si>
+  <si>
+    <t>CONN HEADER R/A 4POS 2.5MM</t>
+  </si>
+  <si>
+    <t>CONN RCA PHONO JACK R/A BLACK</t>
+  </si>
+  <si>
+    <t>LIGHT PIPE PNL MNT 12.7MM LONG</t>
+  </si>
+  <si>
+    <t>492-1154-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bivar-inc/PLP2-500/586464</t>
+  </si>
+  <si>
+    <t>Bivar Inc.</t>
+  </si>
+  <si>
+    <t>PLP2-500</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B4B-XH-AM/1651035</t>
+  </si>
+  <si>
+    <t>455-B4B-XH-AM-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 4POS 2.5MM</t>
+  </si>
+  <si>
+    <t>B4B-XH-AM</t>
+  </si>
+  <si>
+    <t>LM78L05ACZ/LFT1 Texas Instruments | Integrated Circuits (ICs) | DigiKey</t>
+  </si>
+  <si>
+    <t>296-46607-1-ND</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>LM78L05ACZ/LFT1</t>
+  </si>
+  <si>
+    <t>5.0V</t>
+  </si>
+  <si>
+    <t>PTR030V0110-BK Eaton - Electronics Division | Circuit Protection | DigiKey</t>
+  </si>
+  <si>
+    <t>PTR030V0110-BK-ND</t>
+  </si>
+  <si>
+    <t>Eaton - Electronics Division</t>
+  </si>
+  <si>
+    <t>PTR030V0110-BK</t>
+  </si>
+  <si>
+    <t>1.1A</t>
+  </si>
+  <si>
+    <t>PTC RESET FUSE 30V 1.1A RADIAL</t>
+  </si>
+  <si>
+    <t>118-PV36W103C01B00-ND</t>
+  </si>
+  <si>
+    <t>PV36W103C01B00 Bourns Inc. | Potentiometers, Variable Resistors | DigiKey</t>
+  </si>
+  <si>
+    <t>PV36W103C01B00</t>
+  </si>
+  <si>
+    <t>TRIMMER 10K OHM 0.5W PC PIN TOP</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>TRANS 8NPN DARL 50V 0.5A 18DIP</t>
+  </si>
+  <si>
+    <t>ULN2803A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/ULN2803A/599591</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/onsemi/1N914BTR/458816</t>
+  </si>
+  <si>
+    <t>1N914BCT-ND</t>
+  </si>
+  <si>
+    <t>onsemi</t>
+  </si>
+  <si>
+    <t>1N914BTR</t>
+  </si>
+  <si>
+    <t>DIODE STANDARD 100V 200MA DO35</t>
+  </si>
+  <si>
+    <t>3-pin header, 2.54mm pitch</t>
+  </si>
+  <si>
+    <t>CFR-25JB-52-1K YAGEO | Resistors | DigiKey</t>
+  </si>
+  <si>
+    <t>1.0KQBK-ND</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>CFR-25JB-52-1K</t>
+  </si>
+  <si>
+    <t>RES 1K OHM 5% 1/4W AXIAL</t>
+  </si>
+  <si>
+    <t>DO NOT INSTALL - pads have shorting trace</t>
+  </si>
+  <si>
+    <t>1N4007RLGOSCT-ND</t>
+  </si>
+  <si>
+    <t>1N4007RLG</t>
+  </si>
+  <si>
+    <t>DIODE STANDARD 1000V 1A AXIAL</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/onsemi/1N4007RLG/918021</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B07LCCLCFF</t>
+  </si>
+  <si>
+    <t>uxcell</t>
+  </si>
+  <si>
+    <t>B07LCCLCFF</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0CKXJLP4B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESP32-S3-DevKitC-1 N16R8 </t>
+  </si>
+  <si>
+    <t>ESP32-S3-DevKitC-1 N16R8 or N8</t>
+  </si>
+  <si>
+    <t>B0CKXJLP4B</t>
+  </si>
+  <si>
+    <t>DORHEA</t>
+  </si>
+  <si>
+    <t>B077D1NY4T</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B077D1NY4T</t>
+  </si>
+  <si>
+    <t>CESS ENTERPRISE</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0739RYXVC</t>
+  </si>
+  <si>
+    <t>‎US-EL-CP-009</t>
+  </si>
+  <si>
+    <t>ELEGOO</t>
+  </si>
+  <si>
+    <t>B0739RYXVC</t>
+  </si>
+  <si>
+    <t>CONN JACK R/A PCB 5.5X2.1MM</t>
+  </si>
+  <si>
+    <t>54-00166</t>
+  </si>
+  <si>
+    <t>Tensility International Corp</t>
+  </si>
+  <si>
+    <t>839-54-00166-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cornell-dubilier-knowles/226CKR050M/5411619</t>
+  </si>
+  <si>
+    <t>1572-1384-ND</t>
+  </si>
+  <si>
+    <t>Cornell Dubilier Knowles</t>
+  </si>
+  <si>
+    <t>226CKR050M</t>
+  </si>
+  <si>
+    <t>CAP ALUM 22UF 20% 50V RADIAL TH</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tensility-international-corp/54-00166/10459294</t>
+  </si>
+  <si>
+    <t>0.1 µF ±1% 50V Ceramic Capacitor C0G, NP0 Radial</t>
+  </si>
+  <si>
+    <t>C333C104F5G5TA</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>C333C104F5G5TA-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kemet/C333C104F5G5TA/6658919</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,6 +531,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0F1111"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -455,13 +560,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -803,25 +916,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
     <col min="7" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="45.85546875" customWidth="1"/>
+    <col min="9" max="9" width="48.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -849,15 +963,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1">
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
@@ -865,640 +979,727 @@
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
+      <c r="F2" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>98</v>
+        <v>158</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" t="s">
+        <v>153</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>28</v>
+      <c r="G7" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>107</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+        <v>105</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>31</v>
+      <c r="A9" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>12</v>
+        <v>95</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>36</v>
+      <c r="A10" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>12</v>
+        <v>81</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>41</v>
+      <c r="A11" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>12</v>
+        <v>85</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>45</v>
+      <c r="A12" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>133</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>49</v>
+        <v>133</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>12</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>50</v>
+      <c r="A13" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>51</v>
+        <v>133</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>12</v>
+        <v>143</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>55</v>
+      <c r="A14" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>56</v>
+        <v>147</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>12</v>
+        <v>149</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>55</v>
+      <c r="A15" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="B15" s="1">
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>56</v>
+        <v>147</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>12</v>
+        <v>149</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>55</v>
+      <c r="A16" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>56</v>
+        <v>147</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>12</v>
+        <v>149</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>59</v>
+      <c r="A17" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>60</v>
+        <v>128</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>12</v>
+        <v>125</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>65</v>
+      <c r="A18" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="B18" s="1">
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>69</v>
+        <v>133</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>12</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>71</v>
+      <c r="A19" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>130</v>
+        <v>78</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>131</v>
+        <v>79</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>127</v>
+        <v>75</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>128</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>73</v>
+      <c r="A20" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>78</v>
+        <v>99</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
         <v>19</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="1">
+      <c r="B22">
         <v>2</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>12</v>
+      <c r="C22" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>86</v>
+      <c r="A23" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>87</v>
+        <v>133</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>91</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>12</v>
+        <v>79</v>
+      </c>
+      <c r="H24" t="s">
+        <v>109</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>19</v>
+      <c r="A25" s="6">
+        <v>22</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="F25" s="1" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>124</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" t="s">
+        <v>93</v>
+      </c>
+      <c r="G26" t="s">
+        <v>92</v>
+      </c>
+      <c r="H26" t="s">
+        <v>90</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I25" r:id="rId1" xr:uid="{B776064C-F2A1-4953-93C2-6F073EE9DD73}"/>
     <hyperlink ref="I19" r:id="rId2" xr:uid="{C2D78EDF-2CFA-4D28-BEA4-1A81F2A1B380}"/>
+    <hyperlink ref="I10" r:id="rId3" xr:uid="{F9A76EB3-61BA-4453-91AF-16354993D3DD}"/>
+    <hyperlink ref="I11" r:id="rId4" xr:uid="{A9AA7442-707F-42FF-A437-B11B692A2150}"/>
+    <hyperlink ref="I26" r:id="rId5" xr:uid="{40C7A023-818C-4F76-A10C-34C33F1DF3B9}"/>
+    <hyperlink ref="I9" r:id="rId6" xr:uid="{4355BB90-B48B-485D-A89A-5B6749399CED}"/>
+    <hyperlink ref="I20" r:id="rId7" display="https://www.digikey.com/en/products/detail/texas-instruments/LM78L05ACZ-LFT1/3640754" xr:uid="{C9A02BB5-93FF-44F0-BFB1-40EF5E630FAF}"/>
+    <hyperlink ref="I8" r:id="rId8" display="https://www.digikey.com/en/products/detail/eaton-electronics-division/PTR030V0110-BK/2675229" xr:uid="{FB932F30-6EF4-46B5-B730-8F3FA0A5AAEA}"/>
+    <hyperlink ref="I24" r:id="rId9" display="https://www.digikey.com/en/products/detail/bourns-inc/PV36W103C01B00/666502" xr:uid="{3B1F33F3-7644-487C-9C6B-9A6447C25617}"/>
+    <hyperlink ref="I22" r:id="rId10" xr:uid="{13A2F7B0-D29B-4D06-BC8C-BC0D8A2DF6C5}"/>
+    <hyperlink ref="I5" r:id="rId11" xr:uid="{6F537FDF-792A-4C77-9A28-12F9D7912276}"/>
+    <hyperlink ref="I17" r:id="rId12" display="https://www.digikey.com/en/products/detail/yageo/cfr-25jb-52-1k/96" xr:uid="{03260487-744D-40E9-B1F0-D83C843C5D78}"/>
+    <hyperlink ref="I4" r:id="rId13" xr:uid="{D0AAFA75-6917-4DA3-9B21-7663B2BF9D01}"/>
+    <hyperlink ref="I7" r:id="rId14" xr:uid="{F9CF57DD-D937-4BC9-918D-18D8C5610A3F}"/>
+    <hyperlink ref="I21" r:id="rId15" xr:uid="{EF43E3B6-86CF-4067-8D83-ABC28265DDEA}"/>
+    <hyperlink ref="I13" r:id="rId16" xr:uid="{5EAE351E-0771-4625-B763-9066049AE545}"/>
+    <hyperlink ref="I14" r:id="rId17" xr:uid="{2D150487-9E43-4E84-91E1-CBDB3059AC1E}"/>
+    <hyperlink ref="I16" r:id="rId18" xr:uid="{65517817-13BD-4CB3-9563-FFA14794DDA6}"/>
+    <hyperlink ref="I15" r:id="rId19" xr:uid="{15A1867F-DC53-40F6-89CE-82018E7F24BF}"/>
+    <hyperlink ref="I6" r:id="rId20" xr:uid="{D073F544-81F1-4B59-ACEC-FD84F94A12AF}"/>
+    <hyperlink ref="I3" r:id="rId21" xr:uid="{50E8EB31-88EC-444D-9CD3-BFF64651CD1A}"/>
+    <hyperlink ref="I2" r:id="rId22" xr:uid="{45E1E599-08F2-49D9-8EFA-B2EA383C4EC2}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added cables and plug
</commit_message>
<xml_diff>
--- a/PCB_files/IC905_Band_Decoder_BOM-20-Jan-2025.xlsx
+++ b/PCB_files/IC905_Band_Decoder_BOM-20-Jan-2025.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="191" documentId="8_{48654F1B-A63E-4FD9-B4DB-5299DF6E0C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D691DDEA-53B8-4B1C-A413-5281C816FA8F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5578E9D6-5077-48CE-9232-2E67F6738419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="2625" windowWidth="24420" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28830" yWindow="1095" windowWidth="21600" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_905_Band_Decoder_Band_Decod" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="177">
   <si>
     <t>No.</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Manufacturer</t>
   </si>
   <si>
-    <t>Supplier Part</t>
-  </si>
-  <si>
     <t>Supplier</t>
   </si>
   <si>
@@ -510,13 +507,52 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/kemet/C333C104F5G5TA/6658919</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0BXX1L8G7</t>
+  </si>
+  <si>
+    <t>B0BXX1L8G7</t>
+  </si>
+  <si>
+    <t>Supplier Part# or Amazon ASIN</t>
+  </si>
+  <si>
+    <t>CableCreation</t>
+  </si>
+  <si>
+    <t>Black TPU</t>
+  </si>
+  <si>
+    <t>Short Micro USB to USB C Cable 0.65 FT (2-pack)</t>
+  </si>
+  <si>
+    <t>6" stereo 1/8" phone plug to RCA plug</t>
+  </si>
+  <si>
+    <t>6" Dc plug to DC plug (2.1x5.5mm at both ends)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B09PN43RHQ</t>
+  </si>
+  <si>
+    <t>Male VGA Solderless Quick Connector 16mm Thinner (2-pack)</t>
+  </si>
+  <si>
+    <t>B09PN43RHQ</t>
+  </si>
+  <si>
+    <t>ANMBEST</t>
+  </si>
+  <si>
+    <t>DIY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,6 +571,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0F1111"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -560,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -576,6 +618,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -916,10 +959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,7 +977,7 @@
     <col min="9" max="9" width="48.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -957,588 +1000,588 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" t="s">
         <v>151</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>152</v>
       </c>
-      <c r="H6" t="s">
-        <v>153</v>
-      </c>
       <c r="I6" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>137</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H13" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="I14" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1">
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="I15" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="I16" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1">
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="E19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="H19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="1">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="1">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="E21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="I21" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1549,78 +1592,78 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="D22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="1">
-        <v>1</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H24" t="s">
+        <v>108</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1631,23 +1674,23 @@
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1658,22 +1701,99 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26" t="s">
+        <v>91</v>
+      </c>
+      <c r="H26" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F26" t="s">
-        <v>93</v>
-      </c>
-      <c r="G26" t="s">
-        <v>92</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="I26" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="I26" s="3" t="s">
-        <v>91</v>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>169</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G27" t="s">
+        <v>167</v>
+      </c>
+      <c r="H27" t="s">
+        <v>165</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1700,6 +1820,8 @@
     <hyperlink ref="I6" r:id="rId20" xr:uid="{D073F544-81F1-4B59-ACEC-FD84F94A12AF}"/>
     <hyperlink ref="I3" r:id="rId21" xr:uid="{50E8EB31-88EC-444D-9CD3-BFF64651CD1A}"/>
     <hyperlink ref="I2" r:id="rId22" xr:uid="{45E1E599-08F2-49D9-8EFA-B2EA383C4EC2}"/>
+    <hyperlink ref="I27" r:id="rId23" xr:uid="{1BBE951E-833C-4EBC-8C28-762BA476C638}"/>
+    <hyperlink ref="I30" r:id="rId24" xr:uid="{7289FDA1-35DC-4069-9EBF-216859C3C9E7}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>